<commit_message>
working on dual lcr
</commit_message>
<xml_diff>
--- a/examples/dual-analysis/dual-database.xlsx
+++ b/examples/dual-analysis/dual-database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cudmore/Sites/SanPy/examples/dual-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C506767B-D679-5546-BC75-B8144C08F734}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A565B196-FCFB-5F48-921D-A6B9938FEDCE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="460" windowWidth="27360" windowHeight="14680" xr2:uid="{8E007D05-730B-B14A-AC67-EF192B0933CD}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="27360" windowHeight="14680" xr2:uid="{8E007D05-730B-B14A-AC67-EF192B0933CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="110">
   <si>
     <t>data path</t>
   </si>
@@ -331,6 +331,36 @@
   </si>
   <si>
     <t>vmThreshold</t>
+  </si>
+  <si>
+    <t>numLines</t>
+  </si>
+  <si>
+    <t>numPixels</t>
+  </si>
+  <si>
+    <t>umLength</t>
+  </si>
+  <si>
+    <t>umPerPixel</t>
+  </si>
+  <si>
+    <t>totalSeconds</t>
+  </si>
+  <si>
+    <t>secondsPerLine</t>
+  </si>
+  <si>
+    <t>linesPerSecond</t>
+  </si>
+  <si>
+    <t>firstFrameSeconds</t>
+  </si>
+  <si>
+    <t>xMaxRecordingSec</t>
+  </si>
+  <si>
+    <t>meh_later</t>
   </si>
 </sst>
 </file>
@@ -738,10 +768,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD968B9-DDA8-7A49-B49C-B3EBA0FD8938}">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:AG22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane xSplit="10620" topLeftCell="Y1" activePane="topRight"/>
+      <selection activeCell="D13" sqref="A13:XFD13"/>
+      <selection pane="topRight" activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -759,9 +791,11 @@
     <col min="17" max="17" width="12.83203125" style="8" customWidth="1"/>
     <col min="18" max="22" width="10.83203125" style="8"/>
     <col min="23" max="23" width="10.83203125" style="9"/>
+    <col min="28" max="28" width="10.83203125" style="9"/>
+    <col min="31" max="31" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -834,8 +868,35 @@
       <c r="X1" t="s">
         <v>62</v>
       </c>
+      <c r="Y1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -869,8 +930,35 @@
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
+      <c r="Y2">
+        <v>10000</v>
+      </c>
+      <c r="Z2">
+        <v>138</v>
+      </c>
+      <c r="AA2">
+        <v>57.176000000000002</v>
+      </c>
+      <c r="AB2" s="9">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="AC2">
+        <v>35.496000000000002</v>
+      </c>
+      <c r="AD2">
+        <v>3.5496E-3</v>
+      </c>
+      <c r="AE2" s="9">
+        <v>281.72188415596099</v>
+      </c>
+      <c r="AF2">
+        <v>0.51529999999999998</v>
+      </c>
+      <c r="AG2">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>1</v>
@@ -901,8 +989,35 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
+      <c r="Y3">
+        <v>10000</v>
+      </c>
+      <c r="Z3">
+        <v>146</v>
+      </c>
+      <c r="AA3">
+        <v>60.491</v>
+      </c>
+      <c r="AB3" s="9">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="AC3">
+        <v>36.295999999999999</v>
+      </c>
+      <c r="AD3">
+        <v>3.6295999999999902E-3</v>
+      </c>
+      <c r="AE3" s="9">
+        <v>275.51245316288299</v>
+      </c>
+      <c r="AF3">
+        <v>0.51539999999999997</v>
+      </c>
+      <c r="AG3">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>2</v>
@@ -964,8 +1079,35 @@
       <c r="X4" s="8">
         <v>0.5</v>
       </c>
+      <c r="Y4">
+        <v>7000</v>
+      </c>
+      <c r="Z4">
+        <v>208</v>
+      </c>
+      <c r="AA4">
+        <v>172.357</v>
+      </c>
+      <c r="AB4" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC4">
+        <v>29.745999999999999</v>
+      </c>
+      <c r="AD4">
+        <v>4.2494285714285698E-3</v>
+      </c>
+      <c r="AE4" s="9">
+        <v>235.32575808511999</v>
+      </c>
+      <c r="AF4">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="AG4">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>3</v>
@@ -1025,8 +1167,35 @@
       <c r="X5" s="8">
         <v>0.5</v>
       </c>
+      <c r="Y5">
+        <v>7000</v>
+      </c>
+      <c r="Z5">
+        <v>208</v>
+      </c>
+      <c r="AA5">
+        <v>172.357</v>
+      </c>
+      <c r="AB5" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC5">
+        <v>29.745999999999999</v>
+      </c>
+      <c r="AD5">
+        <v>4.2494285714285698E-3</v>
+      </c>
+      <c r="AE5" s="9">
+        <v>235.32575808511999</v>
+      </c>
+      <c r="AF5">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="AG5">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>4</v>
@@ -1086,8 +1255,35 @@
       <c r="X6" s="8">
         <v>0.5</v>
       </c>
+      <c r="Y6">
+        <v>12000</v>
+      </c>
+      <c r="Z6">
+        <v>208</v>
+      </c>
+      <c r="AA6">
+        <v>172.357</v>
+      </c>
+      <c r="AB6" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC6">
+        <v>50.996000000000002</v>
+      </c>
+      <c r="AD6">
+        <v>4.2496666666666603E-3</v>
+      </c>
+      <c r="AE6" s="9">
+        <v>235.31257353517901</v>
+      </c>
+      <c r="AF6">
+        <v>0.90659999999999996</v>
+      </c>
+      <c r="AG6">
+        <v>49.999899999999997</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>5</v>
@@ -1120,8 +1316,35 @@
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
+      <c r="Y7">
+        <v>7000</v>
+      </c>
+      <c r="Z7">
+        <v>174</v>
+      </c>
+      <c r="AA7">
+        <v>144.18299999999999</v>
+      </c>
+      <c r="AB7" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC7">
+        <v>27.366</v>
+      </c>
+      <c r="AD7">
+        <v>3.9094285714285698E-3</v>
+      </c>
+      <c r="AE7" s="9">
+        <v>255.79185851055999</v>
+      </c>
+      <c r="AF7">
+        <v>0.51570000000000005</v>
+      </c>
+      <c r="AG7">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>6</v>
@@ -1152,8 +1375,35 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
+      <c r="Y8">
+        <v>7000</v>
+      </c>
+      <c r="Z8">
+        <v>174</v>
+      </c>
+      <c r="AA8">
+        <v>144.18299999999999</v>
+      </c>
+      <c r="AB8" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC8">
+        <v>27.366</v>
+      </c>
+      <c r="AD8">
+        <v>3.9094285714285698E-3</v>
+      </c>
+      <c r="AE8" s="9">
+        <v>255.79185851055999</v>
+      </c>
+      <c r="AF8">
+        <v>0.51570000000000005</v>
+      </c>
+      <c r="AG8">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>7</v>
@@ -1186,8 +1436,35 @@
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
+      <c r="Y9">
+        <v>8000</v>
+      </c>
+      <c r="Z9">
+        <v>151</v>
+      </c>
+      <c r="AA9">
+        <v>125.125</v>
+      </c>
+      <c r="AB9" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC9">
+        <v>29.515999999999998</v>
+      </c>
+      <c r="AD9">
+        <v>3.6894999999999901E-3</v>
+      </c>
+      <c r="AE9" s="9">
+        <v>271.03943623797198</v>
+      </c>
+      <c r="AF9">
+        <v>0.51549999999999996</v>
+      </c>
+      <c r="AG9">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>8</v>
@@ -1247,8 +1524,35 @@
       <c r="X10" s="8">
         <v>0.5</v>
       </c>
+      <c r="Y10">
+        <v>8000</v>
+      </c>
+      <c r="Z10">
+        <v>151</v>
+      </c>
+      <c r="AA10">
+        <v>125.125</v>
+      </c>
+      <c r="AB10" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC10">
+        <v>29.515999999999998</v>
+      </c>
+      <c r="AD10">
+        <v>3.6894999999999901E-3</v>
+      </c>
+      <c r="AE10" s="9">
+        <v>271.03943623797198</v>
+      </c>
+      <c r="AF10">
+        <v>0.51549999999999996</v>
+      </c>
+      <c r="AG10">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>9</v>
@@ -1308,8 +1612,35 @@
       <c r="X11" s="8">
         <v>0.5</v>
       </c>
+      <c r="Y11">
+        <v>8000</v>
+      </c>
+      <c r="Z11">
+        <v>151</v>
+      </c>
+      <c r="AA11">
+        <v>125.125</v>
+      </c>
+      <c r="AB11" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC11">
+        <v>29.515999999999998</v>
+      </c>
+      <c r="AD11">
+        <v>3.6894999999999901E-3</v>
+      </c>
+      <c r="AE11" s="9">
+        <v>271.03943623797198</v>
+      </c>
+      <c r="AF11">
+        <v>0.51549999999999996</v>
+      </c>
+      <c r="AG11">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>10</v>
@@ -1348,8 +1679,35 @@
       <c r="P12" s="6">
         <v>-20</v>
       </c>
+      <c r="Y12">
+        <v>20000</v>
+      </c>
+      <c r="Z12">
+        <v>26</v>
+      </c>
+      <c r="AA12">
+        <v>21.545000000000002</v>
+      </c>
+      <c r="AB12" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC12">
+        <v>27.399000000000001</v>
+      </c>
+      <c r="AD12">
+        <v>1.36995E-3</v>
+      </c>
+      <c r="AE12" s="9">
+        <v>729.95364794335501</v>
+      </c>
+      <c r="AF12">
+        <v>0.51280000000000003</v>
+      </c>
+      <c r="AG12">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>11</v>
@@ -1400,8 +1758,35 @@
       <c r="U13" s="8">
         <v>250</v>
       </c>
+      <c r="Y13">
+        <v>7000</v>
+      </c>
+      <c r="Z13">
+        <v>163</v>
+      </c>
+      <c r="AA13">
+        <v>135.06800000000001</v>
+      </c>
+      <c r="AB13" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC13">
+        <v>26.666</v>
+      </c>
+      <c r="AD13">
+        <v>3.8094285714285699E-3</v>
+      </c>
+      <c r="AE13" s="9">
+        <v>262.506562664066</v>
+      </c>
+      <c r="AF13">
+        <v>0.51559999999999995</v>
+      </c>
+      <c r="AG13">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>12</v>
@@ -1432,8 +1817,35 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
+      <c r="Y14">
+        <v>163</v>
+      </c>
+      <c r="Z14">
+        <v>163</v>
+      </c>
+      <c r="AA14">
+        <v>135.06800000000001</v>
+      </c>
+      <c r="AB14" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC14">
+        <v>26.666</v>
+      </c>
+      <c r="AD14">
+        <v>0.16359509202453901</v>
+      </c>
+      <c r="AE14" s="9">
+        <v>6.1126528163204004</v>
+      </c>
+      <c r="AF14">
+        <v>0.51559999999999995</v>
+      </c>
+      <c r="AG14">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>13</v>
@@ -1468,8 +1880,35 @@
       <c r="N15" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="Y15">
+        <v>8000</v>
+      </c>
+      <c r="Z15">
+        <v>180</v>
+      </c>
+      <c r="AA15">
+        <v>149.155</v>
+      </c>
+      <c r="AB15" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC15">
+        <v>31.756</v>
+      </c>
+      <c r="AD15">
+        <v>3.9694999999999999E-3</v>
+      </c>
+      <c r="AE15" s="9">
+        <v>251.920896838392</v>
+      </c>
+      <c r="AF15">
+        <v>0.51570000000000005</v>
+      </c>
+      <c r="AG15">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>14</v>
@@ -1531,8 +1970,35 @@
       <c r="X16" s="8">
         <v>0.5</v>
       </c>
+      <c r="Y16">
+        <v>8000</v>
+      </c>
+      <c r="Z16">
+        <v>180</v>
+      </c>
+      <c r="AA16">
+        <v>149.155</v>
+      </c>
+      <c r="AB16" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC16">
+        <v>31.756</v>
+      </c>
+      <c r="AD16">
+        <v>3.9694999999999999E-3</v>
+      </c>
+      <c r="AE16" s="9">
+        <v>251.920896838392</v>
+      </c>
+      <c r="AF16">
+        <v>0.51570000000000005</v>
+      </c>
+      <c r="AG16">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="17" spans="1:21" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>15</v>
@@ -1583,8 +2049,35 @@
       <c r="U17" s="8">
         <v>250</v>
       </c>
+      <c r="Y17">
+        <v>8000</v>
+      </c>
+      <c r="Z17">
+        <v>157</v>
+      </c>
+      <c r="AA17">
+        <v>130.09700000000001</v>
+      </c>
+      <c r="AB17" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC17">
+        <v>29.995999999999999</v>
+      </c>
+      <c r="AD17">
+        <v>3.7494999999999998E-3</v>
+      </c>
+      <c r="AE17" s="9">
+        <v>266.70222696359502</v>
+      </c>
+      <c r="AF17">
+        <v>0.51549999999999996</v>
+      </c>
+      <c r="AG17">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="18" spans="1:21" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>16</v>
@@ -1635,8 +2128,35 @@
       <c r="U18" s="8">
         <v>250</v>
       </c>
+      <c r="Y18">
+        <v>8000</v>
+      </c>
+      <c r="Z18">
+        <v>157</v>
+      </c>
+      <c r="AA18">
+        <v>130.09700000000001</v>
+      </c>
+      <c r="AB18" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC18">
+        <v>29.995999999999999</v>
+      </c>
+      <c r="AD18">
+        <v>3.7494999999999998E-3</v>
+      </c>
+      <c r="AE18" s="9">
+        <v>266.70222696359502</v>
+      </c>
+      <c r="AF18">
+        <v>0.51549999999999996</v>
+      </c>
+      <c r="AG18">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="19" spans="1:21" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>17</v>
@@ -1669,8 +2189,35 @@
       <c r="N19" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="Y19">
+        <v>9000</v>
+      </c>
+      <c r="Z19">
+        <v>96</v>
+      </c>
+      <c r="AA19">
+        <v>79.55</v>
+      </c>
+      <c r="AB19" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC19">
+        <v>28.167000000000002</v>
+      </c>
+      <c r="AD19">
+        <v>3.1296666666666599E-3</v>
+      </c>
+      <c r="AE19" s="9">
+        <v>319.52284588347999</v>
+      </c>
+      <c r="AF19">
+        <v>0.51490000000000002</v>
+      </c>
+      <c r="AG19">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="20" spans="1:21" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>18</v>
@@ -1682,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="F20" s="1">
         <v>20210129</v>
@@ -1728,8 +2275,35 @@
       <c r="U20" s="8">
         <v>250</v>
       </c>
+      <c r="Y20">
+        <v>9000</v>
+      </c>
+      <c r="Z20">
+        <v>96</v>
+      </c>
+      <c r="AA20">
+        <v>79.55</v>
+      </c>
+      <c r="AB20" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC20">
+        <v>28.167000000000002</v>
+      </c>
+      <c r="AD20">
+        <v>3.1296666666666599E-3</v>
+      </c>
+      <c r="AE20" s="9">
+        <v>319.52284588347999</v>
+      </c>
+      <c r="AF20">
+        <v>0.51490000000000002</v>
+      </c>
+      <c r="AG20">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="21" spans="1:21" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>19</v>
@@ -1780,8 +2354,35 @@
       <c r="U21" s="8">
         <v>500</v>
       </c>
+      <c r="Y21">
+        <v>9000</v>
+      </c>
+      <c r="Z21">
+        <v>147</v>
+      </c>
+      <c r="AA21">
+        <v>121.81</v>
+      </c>
+      <c r="AB21" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC21">
+        <v>32.845999999999997</v>
+      </c>
+      <c r="AD21">
+        <v>3.64955555555555E-3</v>
+      </c>
+      <c r="AE21" s="9">
+        <v>274.00596724106401</v>
+      </c>
+      <c r="AF21">
+        <v>0.51539999999999997</v>
+      </c>
+      <c r="AG21">
+        <v>24.9999</v>
+      </c>
     </row>
-    <row r="22" spans="1:21" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>20</v>
@@ -1834,8 +2435,36 @@
       <c r="U22" s="8">
         <v>500</v>
       </c>
+      <c r="Y22">
+        <v>9000</v>
+      </c>
+      <c r="Z22">
+        <v>75</v>
+      </c>
+      <c r="AA22">
+        <v>62.148000000000003</v>
+      </c>
+      <c r="AB22" s="9">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AC22">
+        <v>26.367000000000001</v>
+      </c>
+      <c r="AD22">
+        <v>2.9296666666666599E-3</v>
+      </c>
+      <c r="AE22" s="9">
+        <v>341.33576060985303</v>
+      </c>
+      <c r="AF22">
+        <v>0.51470000000000005</v>
+      </c>
+      <c r="AG22">
+        <v>24.9999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
going to implement QSplitter
</commit_message>
<xml_diff>
--- a/examples/dual-analysis/dual-database.xlsx
+++ b/examples/dual-analysis/dual-database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cudmore/Sites/SanPy/examples/dual-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134A44FC-FB7B-0842-B2FE-BAE6949C6FEF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCBF5CE-0CDC-BB42-9DDE-CABA42DE6E6C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="740" windowWidth="27360" windowHeight="15760" xr2:uid="{8E007D05-730B-B14A-AC67-EF192B0933CD}"/>
   </bookViews>
@@ -565,7 +565,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -584,6 +584,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -597,7 +603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -614,6 +620,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -930,25 +937,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD968B9-DDA8-7A49-B49C-B3EBA0FD8938}">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <pane xSplit="26780" ySplit="820" topLeftCell="X14" activePane="bottomLeft"/>
-      <selection activeCell="X1" sqref="X1:AF1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="26780" ySplit="820" topLeftCell="X13" activePane="bottomLeft"/>
+      <selection activeCell="L1" sqref="L1:N1048576"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="V17" sqref="V17"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
       <selection pane="bottomRight" activeCell="AB22" sqref="AB22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="12.33203125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="8" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="12" max="13" width="0.1640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
+    <col min="8" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" customWidth="1"/>
+    <col min="13" max="13" width="0.1640625" customWidth="1"/>
     <col min="14" max="14" width="15.5" customWidth="1"/>
     <col min="15" max="15" width="12.83203125" style="6" customWidth="1"/>
     <col min="16" max="16" width="12.83203125" style="8" customWidth="1"/>
@@ -2444,7 +2452,7 @@
       </c>
     </row>
     <row r="21" spans="1:32" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="1">
         <v>19</v>
       </c>

</xml_diff>